<commit_message>
2025 close to final data input. K. Courtney entered the missing KTN 2023 survey data so that was deleted from dataimport. Removed previous year files
</commit_message>
<xml_diff>
--- a/output/KTN_cohosurveytable_1987-2025.xlsx
+++ b/output/KTN_cohosurveytable_1987-2025.xlsx
@@ -2294,7 +2294,7 @@
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>210</v>
+        <v>346.409246893103</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>140</v>
@@ -2303,19 +2303,19 @@
         <v>2150</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>620</v>
+        <v>100</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>295.162537574381</v>
+        <v>256.340476972615</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>2600</v>
+        <v>470</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>720</v>
+        <v>300</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>70</v>
@@ -2397,7 +2397,7 @@
         <v>290</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>245.384669457003</v>
+        <v>247.328693706137</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>650</v>
@@ -2418,7 +2418,7 @@
         <v>200</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>620.379947410462</v>
+        <v>625.294817048046</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>1600</v>
@@ -2441,328 +2441,333 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C2">
+    <cfRule type="expression" dxfId="0" priority="69">
+      <formula>C2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E2">
     <cfRule type="expression" dxfId="0" priority="68">
-      <formula>C2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E2">
+      <formula>E2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F2">
     <cfRule type="expression" dxfId="0" priority="67">
-      <formula>E2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F2">
+      <formula>F2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G2">
     <cfRule type="expression" dxfId="0" priority="66">
-      <formula>F2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G2">
+      <formula>G2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H2">
     <cfRule type="expression" dxfId="0" priority="65">
-      <formula>G2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H2">
+      <formula>H2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I2">
     <cfRule type="expression" dxfId="0" priority="64">
-      <formula>H2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I2">
+      <formula>I2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J4">
     <cfRule type="expression" dxfId="0" priority="63">
-      <formula>I2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J4">
+      <formula>J4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F5">
     <cfRule type="expression" dxfId="0" priority="62">
-      <formula>J4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F5">
+      <formula>F5&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G5">
     <cfRule type="expression" dxfId="0" priority="61">
-      <formula>F5&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G5">
+      <formula>G5&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I5">
     <cfRule type="expression" dxfId="0" priority="60">
-      <formula>G5&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I5">
+      <formula>I5&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J5">
     <cfRule type="expression" dxfId="0" priority="59">
-      <formula>I5&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J5">
+      <formula>J5&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C12">
     <cfRule type="expression" dxfId="0" priority="58">
-      <formula>J5&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C12">
+      <formula>C12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F12">
     <cfRule type="expression" dxfId="0" priority="57">
-      <formula>C12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F12">
+      <formula>F12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G12">
     <cfRule type="expression" dxfId="0" priority="56">
-      <formula>F12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G12">
+      <formula>G12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H12">
     <cfRule type="expression" dxfId="0" priority="55">
-      <formula>G12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H12">
+      <formula>H12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:J13">
     <cfRule type="expression" dxfId="0" priority="54">
-      <formula>H12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J13:J13">
+      <formula>J13&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16:L16">
     <cfRule type="expression" dxfId="0" priority="53">
-      <formula>J13&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L16:L16">
+      <formula>L16&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16:O16">
     <cfRule type="expression" dxfId="0" priority="52">
-      <formula>L16&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O16:O16">
+      <formula>O16&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C18">
     <cfRule type="expression" dxfId="0" priority="51">
-      <formula>O16&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C18">
+      <formula>C18&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:J18">
     <cfRule type="expression" dxfId="0" priority="50">
-      <formula>C18&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18:J18">
+      <formula>J18&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:C21">
     <cfRule type="expression" dxfId="0" priority="49">
-      <formula>J18&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C21">
+      <formula>C21&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:J21">
     <cfRule type="expression" dxfId="0" priority="48">
-      <formula>C21&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:J21">
+      <formula>J21&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D22">
     <cfRule type="expression" dxfId="0" priority="47">
-      <formula>J21&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D22">
+      <formula>D22&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:J22">
     <cfRule type="expression" dxfId="0" priority="46">
-      <formula>D22&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22:J22">
+      <formula>J22&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22:N22">
     <cfRule type="expression" dxfId="0" priority="45">
-      <formula>J22&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22:N22">
+      <formula>N22&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22:O22">
     <cfRule type="expression" dxfId="0" priority="44">
-      <formula>N22&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O22:O22">
+      <formula>O22&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23:J23">
     <cfRule type="expression" dxfId="0" priority="43">
-      <formula>O22&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J23:J23">
+      <formula>J23&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23:L23">
     <cfRule type="expression" dxfId="0" priority="42">
-      <formula>J23&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L23:L23">
+      <formula>L23&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:B24">
     <cfRule type="expression" dxfId="0" priority="41">
-      <formula>L23&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B24">
+      <formula>B24&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E25">
     <cfRule type="expression" dxfId="0" priority="40">
-      <formula>B24&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E25">
+      <formula>E25&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25:J25">
     <cfRule type="expression" dxfId="0" priority="39">
-      <formula>E25&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25:J25">
+      <formula>J25&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25:O25">
     <cfRule type="expression" dxfId="0" priority="38">
-      <formula>J25&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O25:O25">
+      <formula>O25&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:B26">
     <cfRule type="expression" dxfId="0" priority="37">
-      <formula>O25&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B26">
+      <formula>B26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C26">
     <cfRule type="expression" dxfId="0" priority="36">
-      <formula>B26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C26">
+      <formula>C26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E26">
     <cfRule type="expression" dxfId="0" priority="35">
-      <formula>C26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E26">
+      <formula>E26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:G26">
     <cfRule type="expression" dxfId="0" priority="34">
-      <formula>E26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G26">
+      <formula>G26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26:J26">
     <cfRule type="expression" dxfId="0" priority="33">
-      <formula>G26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J26:J26">
+      <formula>J26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26:L26">
     <cfRule type="expression" dxfId="0" priority="32">
-      <formula>J26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L26:L26">
+      <formula>L26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:O26">
     <cfRule type="expression" dxfId="0" priority="31">
-      <formula>L26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O26:O26">
+      <formula>O26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:E27">
     <cfRule type="expression" dxfId="0" priority="30">
-      <formula>O26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E27">
+      <formula>E27&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:H27">
     <cfRule type="expression" dxfId="0" priority="29">
-      <formula>E27&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:H27">
+      <formula>H27&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:B28">
     <cfRule type="expression" dxfId="0" priority="28">
-      <formula>H27&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28:B28">
+      <formula>B28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C28">
     <cfRule type="expression" dxfId="0" priority="27">
-      <formula>B28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C28">
+      <formula>C28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D28">
     <cfRule type="expression" dxfId="0" priority="26">
-      <formula>C28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D28">
+      <formula>D28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E28">
     <cfRule type="expression" dxfId="0" priority="25">
-      <formula>D28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E28">
+      <formula>E28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:F28">
     <cfRule type="expression" dxfId="0" priority="24">
-      <formula>E28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F28">
+      <formula>F28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:G28">
     <cfRule type="expression" dxfId="0" priority="23">
-      <formula>F28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G28">
+      <formula>G28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H28">
     <cfRule type="expression" dxfId="0" priority="22">
-      <formula>G28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28:H28">
+      <formula>H28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:I28">
     <cfRule type="expression" dxfId="0" priority="21">
-      <formula>H28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I28">
+      <formula>I28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E29">
     <cfRule type="expression" dxfId="0" priority="20">
-      <formula>I28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E29">
+      <formula>E29&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29:G29">
     <cfRule type="expression" dxfId="0" priority="19">
-      <formula>E29&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29:G29">
+      <formula>G29&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N29">
     <cfRule type="expression" dxfId="0" priority="18">
-      <formula>G29&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N29:N29">
+      <formula>N29&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:E30">
     <cfRule type="expression" dxfId="0" priority="17">
-      <formula>N29&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E30">
+      <formula>E30&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:G30">
     <cfRule type="expression" dxfId="0" priority="16">
-      <formula>E30&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30:G30">
+      <formula>G30&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I31">
     <cfRule type="expression" dxfId="0" priority="15">
-      <formula>G30&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I31">
+      <formula>I31&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:C32">
     <cfRule type="expression" dxfId="0" priority="14">
-      <formula>I31&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C32">
+      <formula>C32&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33:G33">
     <cfRule type="expression" dxfId="0" priority="13">
-      <formula>C32&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G33">
+      <formula>G33&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33:N33">
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>G33&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N33:N33">
+      <formula>N33&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E34">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>N33&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34:E34">
+      <formula>E34&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:C36">
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>E34&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36:C36">
+      <formula>C36&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36:E36">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>C36&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36:E36">
+      <formula>E36&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:B37">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>E36&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37:B37">
+      <formula>B37&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37:E37">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>B37&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37:E37">
+      <formula>E37&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37:J37">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>E37&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J37:J37">
+      <formula>J37&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O37:O37">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>J37&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O37:O37">
+      <formula>O37&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:B38">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>O37&lt;&gt;""</formula>
+      <formula>B38&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:G38">

</xml_diff>

<commit_message>
updated to ignore NA values in total_count
</commit_message>
<xml_diff>
--- a/output/KTN_cohosurveytable_1987-2025.xlsx
+++ b/output/KTN_cohosurveytable_1987-2025.xlsx
@@ -2294,7 +2294,7 @@
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>346.409246893103</v>
+        <v>210</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>140</v>
@@ -2303,19 +2303,19 @@
         <v>2150</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>100</v>
+        <v>620</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>256.340476972615</v>
+        <v>295.162537574381</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>470</v>
+        <v>2600</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>300</v>
+        <v>720</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>70</v>
@@ -2397,7 +2397,7 @@
         <v>290</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>247.328693706137</v>
+        <v>245.384669457003</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>650</v>
@@ -2418,7 +2418,7 @@
         <v>200</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>625.294817048046</v>
+        <v>620.379947410462</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>1600</v>
@@ -2441,333 +2441,328 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C2">
-    <cfRule type="expression" dxfId="0" priority="69">
+    <cfRule type="expression" dxfId="0" priority="68">
       <formula>C2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E2">
-    <cfRule type="expression" dxfId="0" priority="68">
+    <cfRule type="expression" dxfId="0" priority="67">
       <formula>E2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F2">
-    <cfRule type="expression" dxfId="0" priority="67">
+    <cfRule type="expression" dxfId="0" priority="66">
       <formula>F2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G2">
-    <cfRule type="expression" dxfId="0" priority="66">
+    <cfRule type="expression" dxfId="0" priority="65">
       <formula>G2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H2">
-    <cfRule type="expression" dxfId="0" priority="65">
+    <cfRule type="expression" dxfId="0" priority="64">
       <formula>H2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I2">
-    <cfRule type="expression" dxfId="0" priority="64">
+    <cfRule type="expression" dxfId="0" priority="63">
       <formula>I2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J4">
-    <cfRule type="expression" dxfId="0" priority="63">
+    <cfRule type="expression" dxfId="0" priority="62">
       <formula>J4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F5">
-    <cfRule type="expression" dxfId="0" priority="62">
+    <cfRule type="expression" dxfId="0" priority="61">
       <formula>F5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G5">
-    <cfRule type="expression" dxfId="0" priority="61">
+    <cfRule type="expression" dxfId="0" priority="60">
       <formula>G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I5">
-    <cfRule type="expression" dxfId="0" priority="60">
+    <cfRule type="expression" dxfId="0" priority="59">
       <formula>I5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J5">
-    <cfRule type="expression" dxfId="0" priority="59">
+    <cfRule type="expression" dxfId="0" priority="58">
       <formula>J5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C12">
-    <cfRule type="expression" dxfId="0" priority="58">
+    <cfRule type="expression" dxfId="0" priority="57">
       <formula>C12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F12">
-    <cfRule type="expression" dxfId="0" priority="57">
+    <cfRule type="expression" dxfId="0" priority="56">
       <formula>F12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G12">
-    <cfRule type="expression" dxfId="0" priority="56">
+    <cfRule type="expression" dxfId="0" priority="55">
       <formula>G12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H12">
-    <cfRule type="expression" dxfId="0" priority="55">
+    <cfRule type="expression" dxfId="0" priority="54">
       <formula>H12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J13">
-    <cfRule type="expression" dxfId="0" priority="54">
+    <cfRule type="expression" dxfId="0" priority="53">
       <formula>J13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L16">
-    <cfRule type="expression" dxfId="0" priority="53">
+    <cfRule type="expression" dxfId="0" priority="52">
       <formula>L16&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16:O16">
-    <cfRule type="expression" dxfId="0" priority="52">
+    <cfRule type="expression" dxfId="0" priority="51">
       <formula>O16&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C18">
-    <cfRule type="expression" dxfId="0" priority="51">
+    <cfRule type="expression" dxfId="0" priority="50">
       <formula>C18&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J18">
-    <cfRule type="expression" dxfId="0" priority="50">
+    <cfRule type="expression" dxfId="0" priority="49">
       <formula>J18&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C21">
-    <cfRule type="expression" dxfId="0" priority="49">
+    <cfRule type="expression" dxfId="0" priority="48">
       <formula>C21&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:J21">
-    <cfRule type="expression" dxfId="0" priority="48">
+    <cfRule type="expression" dxfId="0" priority="47">
       <formula>J21&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:D22">
-    <cfRule type="expression" dxfId="0" priority="47">
+    <cfRule type="expression" dxfId="0" priority="46">
       <formula>D22&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J22">
-    <cfRule type="expression" dxfId="0" priority="46">
+    <cfRule type="expression" dxfId="0" priority="45">
       <formula>J22&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:N22">
-    <cfRule type="expression" dxfId="0" priority="45">
+    <cfRule type="expression" dxfId="0" priority="44">
       <formula>N22&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O22:O22">
-    <cfRule type="expression" dxfId="0" priority="44">
+    <cfRule type="expression" dxfId="0" priority="43">
       <formula>O22&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:J23">
-    <cfRule type="expression" dxfId="0" priority="43">
+    <cfRule type="expression" dxfId="0" priority="42">
       <formula>J23&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23:L23">
-    <cfRule type="expression" dxfId="0" priority="42">
+    <cfRule type="expression" dxfId="0" priority="41">
       <formula>L23&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B24">
-    <cfRule type="expression" dxfId="0" priority="41">
+    <cfRule type="expression" dxfId="0" priority="40">
       <formula>B24&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E25">
-    <cfRule type="expression" dxfId="0" priority="40">
+    <cfRule type="expression" dxfId="0" priority="39">
       <formula>E25&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:J25">
-    <cfRule type="expression" dxfId="0" priority="39">
+    <cfRule type="expression" dxfId="0" priority="38">
       <formula>J25&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O25:O25">
-    <cfRule type="expression" dxfId="0" priority="38">
+    <cfRule type="expression" dxfId="0" priority="37">
       <formula>O25&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B26">
-    <cfRule type="expression" dxfId="0" priority="37">
+    <cfRule type="expression" dxfId="0" priority="36">
       <formula>B26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C26">
-    <cfRule type="expression" dxfId="0" priority="36">
+    <cfRule type="expression" dxfId="0" priority="35">
       <formula>C26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E26">
-    <cfRule type="expression" dxfId="0" priority="35">
+    <cfRule type="expression" dxfId="0" priority="34">
       <formula>E26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G26">
-    <cfRule type="expression" dxfId="0" priority="34">
+    <cfRule type="expression" dxfId="0" priority="33">
       <formula>G26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J26">
-    <cfRule type="expression" dxfId="0" priority="33">
+    <cfRule type="expression" dxfId="0" priority="32">
       <formula>J26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:L26">
-    <cfRule type="expression" dxfId="0" priority="32">
+    <cfRule type="expression" dxfId="0" priority="31">
       <formula>L26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O26:O26">
-    <cfRule type="expression" dxfId="0" priority="31">
+    <cfRule type="expression" dxfId="0" priority="30">
       <formula>O26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:E27">
-    <cfRule type="expression" dxfId="0" priority="30">
+    <cfRule type="expression" dxfId="0" priority="29">
       <formula>E27&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H27">
-    <cfRule type="expression" dxfId="0" priority="29">
+    <cfRule type="expression" dxfId="0" priority="28">
       <formula>H27&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B28">
-    <cfRule type="expression" dxfId="0" priority="28">
+    <cfRule type="expression" dxfId="0" priority="27">
       <formula>B28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C28">
-    <cfRule type="expression" dxfId="0" priority="27">
+    <cfRule type="expression" dxfId="0" priority="26">
       <formula>C28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D28">
-    <cfRule type="expression" dxfId="0" priority="26">
+    <cfRule type="expression" dxfId="0" priority="25">
       <formula>D28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E28">
-    <cfRule type="expression" dxfId="0" priority="25">
+    <cfRule type="expression" dxfId="0" priority="24">
       <formula>E28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F28">
-    <cfRule type="expression" dxfId="0" priority="24">
+    <cfRule type="expression" dxfId="0" priority="23">
       <formula>F28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:G28">
-    <cfRule type="expression" dxfId="0" priority="23">
+    <cfRule type="expression" dxfId="0" priority="22">
       <formula>G28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:H28">
-    <cfRule type="expression" dxfId="0" priority="22">
+    <cfRule type="expression" dxfId="0" priority="21">
       <formula>H28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I28">
-    <cfRule type="expression" dxfId="0" priority="21">
+    <cfRule type="expression" dxfId="0" priority="20">
       <formula>I28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E29">
-    <cfRule type="expression" dxfId="0" priority="20">
+    <cfRule type="expression" dxfId="0" priority="19">
       <formula>E29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G29">
-    <cfRule type="expression" dxfId="0" priority="19">
+    <cfRule type="expression" dxfId="0" priority="18">
       <formula>G29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29:N29">
-    <cfRule type="expression" dxfId="0" priority="18">
+    <cfRule type="expression" dxfId="0" priority="17">
       <formula>N29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E30">
-    <cfRule type="expression" dxfId="0" priority="17">
+    <cfRule type="expression" dxfId="0" priority="16">
       <formula>E30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G30">
-    <cfRule type="expression" dxfId="0" priority="16">
+    <cfRule type="expression" dxfId="0" priority="15">
       <formula>G30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:I31">
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>I31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C32">
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="0" priority="13">
       <formula>C32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G33">
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>G33&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33:N33">
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="0" priority="11">
       <formula>N33&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E34">
-    <cfRule type="expression" dxfId="0" priority="11">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>E34&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C36">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>C36&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E36">
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>E36&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:B37">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>B37&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:E37">
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>E37&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:J37">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>J37&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37:O37">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>O37&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38:B38">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>B38&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:G38">

</xml_diff>